<commit_message>
Manual and AUtomation cases
</commit_message>
<xml_diff>
--- a/Admin/Suppliers/Manual testcases/Copy outlet settings feature should also be available on ZM Admin.xlsx
+++ b/Admin/Suppliers/Manual testcases/Copy outlet settings feature should also be available on ZM Admin.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\Admin\Suppliers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\zm-buyerautomation\Admin\Suppliers\Manual testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{87A29F27-AD6E-4985-8EC7-147707BAC2E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD1380E-EBEF-4E04-BE30-2FCF15D68C8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="945" windowWidth="20730" windowHeight="10095" xr2:uid="{EC6B5429-B8B7-4285-B6FE-19E0F36347CF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{EC6B5429-B8B7-4285-B6FE-19E0F36347CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="43">
   <si>
     <t>SL. No</t>
   </si>
@@ -189,6 +189,54 @@
     <t xml:space="preserve">It get displayed Outlets details </t>
   </si>
   <si>
+    <t xml:space="preserve">It should displayed the selected Check box from the list of outlets </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">It gets displayed </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Successfully copied settings</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Click the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Apply </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>button (button be in blue colour)</t>
+    </r>
+  </si>
+  <si>
+    <t>Apply outlet settings from(new)</t>
+  </si>
+  <si>
     <r>
       <t>1.Click on the</t>
     </r>
@@ -295,98 +343,100 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">                                            5.click on the Select all ,it will be selected all like </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Order</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">(Enable/disable ordering ,Notifications,Minimum order,Delivery schedule &amp; cutoff times and </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CUST_MARKETLIST</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">(Market list)                                              </t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">It should displayed the selected Check box from the list of outlets </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">It gets displayed </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Successfully copied settings</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Click the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Apply </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>button (button be in blue colour)</t>
-    </r>
-  </si>
-  <si>
-    <t>Apply outlet settings from,</t>
+      <t xml:space="preserve">                                                                                        </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Click on the Select all ,it will be selected all like                     </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">*ORDERS </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Enable/disable ordering, Notifications, Minimum order, Delivery schedule &amp; cutoff times and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*MARKETLIST</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : Market list dropdown                                              </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*BUYERS CUSTOM SETTINGS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : Custom names, Custom product codes, Tags                                                                                 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*INVOICES</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : Invoice payment terms, Seleperson, Invoice notes</t>
+    </r>
+  </si>
+  <si>
+    <t>It displayed as expected</t>
   </si>
 </sst>
 </file>
@@ -819,9 +869,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E024CF9C-10DB-4E3D-8C20-81D79757AD97}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -1042,7 +1092,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>9</v>
       </c>
@@ -1053,19 +1103,19 @@
         <v>12</v>
       </c>
       <c r="D10" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="F10" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>37</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>10</v>
       </c>
@@ -1075,24 +1125,47 @@
       <c r="C11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>31</v>
+      <c r="D11" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+    <row r="12" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>